<commit_message>
Fix typo in multiple template schemas
</commit_message>
<xml_diff>
--- a/template_examples/micsss_template.xlsx
+++ b/template_examples/micsss_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7996CD-D0CC-AA40-A08F-EB1DFCA02213}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD4016C-6D4A-3540-AA5A-E33C513BBD34}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="26040" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="26040" windowHeight="13700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="micsss" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -238,9 +238,6 @@
     <t>AR INCUBATION TIME</t>
   </si>
   <si>
-    <t>CIMAC_PARTICPANT_ID</t>
-  </si>
-  <si>
     <t>CIMAC_SAMPLE_ID</t>
   </si>
   <si>
@@ -404,13 +401,16 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>CIMAC_PARTICIPANT_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,6 +438,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -870,7 +876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -950,7 +956,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -982,7 +988,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1014,7 +1020,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1046,7 +1052,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1078,7 +1084,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1110,7 +1116,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1142,7 +1148,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1174,7 +1180,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1206,7 +1212,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1336,16 +1342,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="F15" s="4">
         <v>23487852</v>
@@ -1354,34 +1360,34 @@
         <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K15" s="4" t="s">
+      <c r="L15" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="M15" s="4">
         <v>9.722222222222221E-2</v>
       </c>
       <c r="N15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="P15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="Q15" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="Q15" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="R15" s="4">
         <v>213423</v>
@@ -1396,10 +1402,10 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="V15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="W15" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="W15" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="X15" s="6">
         <v>2.0833333333333332E-2</v>
@@ -1410,16 +1416,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="F16" s="4">
         <v>87354867</v>
@@ -1428,34 +1434,34 @@
         <v>2</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="M16" s="4">
         <v>9.722222222222221E-2</v>
       </c>
       <c r="N16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O16" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="O16" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="P16" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R16" s="4">
         <v>645456</v>
@@ -1464,16 +1470,16 @@
         <v>7656</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U16" s="6">
         <v>6.25E-2</v>
       </c>
       <c r="V16" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="X16" s="6">
         <v>6.25E-2</v>
@@ -2507,8 +2513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X204"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2568,34 +2574,34 @@
         <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -2603,19 +2609,19 @@
         <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="G5" s="7">
         <v>35796</v>
@@ -2624,13 +2630,13 @@
         <v>35797</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
@@ -2638,19 +2644,19 @@
         <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G6" s="7">
         <v>35797</v>
@@ -2659,13 +2665,13 @@
         <v>35797</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
@@ -2673,19 +2679,19 @@
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G7" s="7">
         <v>35798</v>
@@ -2694,13 +2700,13 @@
         <v>35797</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Don't allow missing template columns/rows (#177)
* Make sure all fields in a template schema exist in a template

* Add test to make sure two templates can't be substituted

* Fix typo in multiple template schemas

* Update unexpected column error message

* Bump package version

* Convert unexpected column error to ValidationError
</commit_message>
<xml_diff>
--- a/template_examples/micsss_template.xlsx
+++ b/template_examples/micsss_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7996CD-D0CC-AA40-A08F-EB1DFCA02213}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD4016C-6D4A-3540-AA5A-E33C513BBD34}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="26040" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="26040" windowHeight="13700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="micsss" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -238,9 +238,6 @@
     <t>AR INCUBATION TIME</t>
   </si>
   <si>
-    <t>CIMAC_PARTICPANT_ID</t>
-  </si>
-  <si>
     <t>CIMAC_SAMPLE_ID</t>
   </si>
   <si>
@@ -404,13 +401,16 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>CIMAC_PARTICIPANT_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,6 +438,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -870,7 +876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -950,7 +956,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -982,7 +988,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1014,7 +1020,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1046,7 +1052,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1078,7 +1084,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1110,7 +1116,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1142,7 +1148,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1174,7 +1180,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1206,7 +1212,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1336,16 +1342,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="F15" s="4">
         <v>23487852</v>
@@ -1354,34 +1360,34 @@
         <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K15" s="4" t="s">
+      <c r="L15" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="M15" s="4">
         <v>9.722222222222221E-2</v>
       </c>
       <c r="N15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="P15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="Q15" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="Q15" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="R15" s="4">
         <v>213423</v>
@@ -1396,10 +1402,10 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="V15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="W15" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="W15" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="X15" s="6">
         <v>2.0833333333333332E-2</v>
@@ -1410,16 +1416,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="F16" s="4">
         <v>87354867</v>
@@ -1428,34 +1434,34 @@
         <v>2</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="M16" s="4">
         <v>9.722222222222221E-2</v>
       </c>
       <c r="N16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O16" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="O16" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="P16" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R16" s="4">
         <v>645456</v>
@@ -1464,16 +1470,16 @@
         <v>7656</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U16" s="6">
         <v>6.25E-2</v>
       </c>
       <c r="V16" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="X16" s="6">
         <v>6.25E-2</v>
@@ -2507,8 +2513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X204"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2568,34 +2574,34 @@
         <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -2603,19 +2609,19 @@
         <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="G5" s="7">
         <v>35796</v>
@@ -2624,13 +2630,13 @@
         <v>35797</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
@@ -2638,19 +2644,19 @@
         <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G6" s="7">
         <v>35797</v>
@@ -2659,13 +2665,13 @@
         <v>35797</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
@@ -2673,19 +2679,19 @@
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G7" s="7">
         <v>35798</v>
@@ -2694,13 +2700,13 @@
         <v>35797</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
prism sub root object creation and tests
</commit_message>
<xml_diff>
--- a/template_examples/micsss_template.xlsx
+++ b/template_examples/micsss_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD4016C-6D4A-3540-AA5A-E33C513BBD34}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B65A045-D6C3-FD46-A56C-C68164BD5B2C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="26040" windowHeight="13700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2511,19 +2511,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X204"/>
+  <dimension ref="A1:K204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X1" sqref="L1:X1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+    <col min="2" max="88" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2541,21 +2541,8 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
@@ -2569,7 +2556,7 @@
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2604,7 +2591,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2639,7 +2626,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2674,7 +2661,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2709,47 +2696,47 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>

</xml_diff>